<commit_message>
update sfserver update experiments
</commit_message>
<xml_diff>
--- a/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
+++ b/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1902,158 +1902,248 @@
       <c r="A3">
         <v>2.1236739999999998</v>
       </c>
+      <c r="C3">
+        <v>2.1328719999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
         <v>2.1204730000000001</v>
       </c>
+      <c r="C4">
+        <v>2.1349960000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
         <v>2.120206</v>
       </c>
+      <c r="C5">
+        <v>2.1153960000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
         <v>2.1194839999999999</v>
       </c>
+      <c r="C6">
+        <v>2.182798</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
         <v>2.1188020000000001</v>
       </c>
+      <c r="C7">
+        <v>2.1255259999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
         <v>4</v>
       </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
         <v>4.222334</v>
       </c>
+      <c r="C11">
+        <v>2.1342910000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12">
         <v>4.2081850000000003</v>
       </c>
+      <c r="C12">
+        <v>2.1290909999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13">
         <v>4.2201599999999999</v>
       </c>
+      <c r="C13">
+        <v>2.1300340000000002</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
         <v>4.2083240000000002</v>
       </c>
+      <c r="C14">
+        <v>2.12243</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
         <v>4.2107270000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C15">
+        <v>2.1209600000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>8.3901690000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="C20">
+        <v>2.140355</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>8.3857809999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="C21">
+        <v>2.1380560000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>8.3821349999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="C22">
+        <v>2.139481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>8.3843169999999994</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="C23">
+        <v>2.1326369999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>8.3885059999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="C24">
+        <v>2.1319370000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="C27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>16.752087</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="C28">
+        <v>2.1677909999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>16.754024999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C29">
+        <v>2.1599439999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>16.754795000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="C30">
+        <v>2.1534990000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>16.748601000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31">
+        <v>2.149159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>16.758751</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="C32">
+        <v>2.1557819999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="C36">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>33.522022</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="C37">
+        <v>2.2002830000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>33.475338000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="C38">
+        <v>2.1922450000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>33.463346000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="C39">
+        <v>2.1933370000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>33.461804999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="C40">
+        <v>2.1951710000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>33.472478000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="C41">
+        <v>2.1929270000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="C46">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>66.939031</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>66.987172999999999</v>
       </c>

</xml_diff>

<commit_message>
update multinode scripts(ok for broadcaster)
</commit_message>
<xml_diff>
--- a/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
+++ b/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="swift" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="respondtime" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">eventdriven!$A$1:$A$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">eventdriven!$A$2:$A$8</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>chained</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,10 +101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">cd </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>publish</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,6 +114,34 @@
   </si>
   <si>
     <t>broadcaster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run every thing on one node (send request by interfaces lo)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eventNotify operator server all on same node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>net.core.somaxconn = 1024(sysctl net.core.somaxconn)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check span 1000us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aggregation need to send more event request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> server span 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the sockets number get to the upper limitation(14:Socket closed)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,8 +201,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,7 +419,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="213">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -464,6 +514,19 @@
     <cellStyle name="访问过的超链接" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -557,6 +620,19 @@
     <cellStyle name="超链接" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="211" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1194,7 +1270,7 @@
                   <c:v>4.332162</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.845494</c:v>
+                  <c:v>10.6195504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,7 +1642,7 @@
                   <c:v>4.062134</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.337818</c:v>
+                  <c:v>7.1534312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,10 +1755,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>graph!$B$76:$K$76</c:f>
+              <c:f>graph!$B$76:$J$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -1708,20 +1784,17 @@
                   <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$B$77:$K$77</c:f>
+              <c:f>graph!$B$77:$J$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4.226253</c:v>
                 </c:pt>
@@ -1747,10 +1820,7 @@
                   <c:v>5.5248494</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.2896678</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.8032056</c:v>
+                  <c:v>7.306993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1773,10 +1843,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>graph!$B$76:$K$76</c:f>
+              <c:f>graph!$B$76:$J$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -1802,20 +1872,17 @@
                   <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$B$78:$K$78</c:f>
+              <c:f>graph!$B$78:$J$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.067029</c:v>
                 </c:pt>
@@ -1841,10 +1908,7 @@
                   <c:v>2.6043186</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1656578</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.1867572</c:v>
+                  <c:v>3.1429132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1867,10 +1931,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>graph!$B$76:$K$76</c:f>
+              <c:f>graph!$B$76:$J$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -1896,20 +1960,17 @@
                   <c:v>256.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>512.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1024.0</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>graph!$B$79:$K$79</c:f>
+              <c:f>graph!$B$79:$J$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2.120444</c:v>
                 </c:pt>
@@ -1932,13 +1993,10 @@
                   <c:v>2.8306176</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3443094</c:v>
+                  <c:v>4.1016348</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.6314818</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43.9029444</c:v>
+                  <c:v>7.2147716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2025,9 +2083,9 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2055,10 +2113,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2464,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55:H79"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3279,7 +3337,7 @@
         <v>5.3799460000000003</v>
       </c>
       <c r="G68">
-        <v>7.441154</v>
+        <v>6.9235899999999999</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -3290,7 +3348,7 @@
         <v>5.2816219999999996</v>
       </c>
       <c r="G69">
-        <v>7.0254459999999996</v>
+        <v>7.3019509999999999</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3301,7 +3359,7 @@
         <v>5.4723769999999998</v>
       </c>
       <c r="G70">
-        <v>7.3721209999999999</v>
+        <v>7.2900460000000002</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3312,7 +3370,7 @@
         <v>5.350301</v>
       </c>
       <c r="G71">
-        <v>7.1722520000000003</v>
+        <v>7.5084330000000001</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3331,11 +3389,11 @@
         <v>5.3688034</v>
       </c>
       <c r="G72">
-        <v>7.4373659999999999</v>
+        <v>7.5109450000000004</v>
       </c>
       <c r="H72">
         <f>AVERAGE(G68:G72)</f>
-        <v>7.2896677999999993</v>
+        <v>7.3069930000000003</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3441,7 +3499,7 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView topLeftCell="F46" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55:H83"/>
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4252,7 +4310,7 @@
         <v>2.6530770000000001</v>
       </c>
       <c r="G72">
-        <v>3.1178439999999998</v>
+        <v>3.2263419999999998</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -4263,7 +4321,7 @@
         <v>2.7668020000000002</v>
       </c>
       <c r="G73">
-        <v>3.1671559999999999</v>
+        <v>3.0822020000000001</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -4274,7 +4332,7 @@
         <v>2.8087209999999998</v>
       </c>
       <c r="G74">
-        <v>3.1947890000000001</v>
+        <v>3.118026</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -4285,7 +4343,7 @@
         <v>2.6786430000000001</v>
       </c>
       <c r="G75">
-        <v>3.165686</v>
+        <v>3.1582189999999999</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -4304,11 +4362,11 @@
         <v>2.7131100000000004</v>
       </c>
       <c r="G76">
-        <v>3.182814</v>
+        <v>3.1297769999999998</v>
       </c>
       <c r="H76">
         <f>AVERAGE(G72:G76)</f>
-        <v>3.1656578000000004</v>
+        <v>3.1429132000000002</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -4406,967 +4464,992 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60:H85"/>
+    <sheetView topLeftCell="D47" workbookViewId="0">
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
+    <col min="6" max="6" width="53.6640625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>2.1236739999999998</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2.1328719999999999</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2.13436</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>2.1249739999999999</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>2.1204730000000001</v>
+        <v>2.1236739999999998</v>
       </c>
       <c r="C4">
-        <v>2.1349960000000001</v>
+        <v>2.1328719999999999</v>
       </c>
       <c r="E4">
-        <v>2.1237710000000001</v>
+        <v>2.13436</v>
       </c>
       <c r="G4">
-        <v>2.1214759999999999</v>
+        <v>2.1249739999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>2.120206</v>
+        <v>2.1204730000000001</v>
       </c>
       <c r="C5">
-        <v>2.1153960000000001</v>
+        <v>2.1349960000000001</v>
       </c>
       <c r="E5">
-        <v>2.121505</v>
+        <v>2.1237710000000001</v>
       </c>
       <c r="G5">
-        <v>2.1215480000000002</v>
+        <v>2.1214759999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>2.1194839999999999</v>
+        <v>2.120206</v>
       </c>
       <c r="C6">
-        <v>2.182798</v>
+        <v>2.1153960000000001</v>
       </c>
       <c r="E6">
-        <v>2.123964</v>
+        <v>2.121505</v>
       </c>
       <c r="G6">
-        <v>2.1224780000000001</v>
+        <v>2.1215480000000002</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
+        <v>2.1194839999999999</v>
+      </c>
+      <c r="C7">
+        <v>2.182798</v>
+      </c>
+      <c r="E7">
+        <v>2.123964</v>
+      </c>
+      <c r="G7">
+        <v>2.1224780000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
         <v>2.1188020000000001</v>
       </c>
-      <c r="B7">
-        <f>A3:A7</f>
+      <c r="B8">
+        <f>A4:A8</f>
         <v>2.1188020000000001</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>2.1255259999999998</v>
       </c>
-      <c r="D7">
-        <f>C3:C7</f>
+      <c r="D8">
+        <f>C4:C8</f>
         <v>2.1255259999999998</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>2.1216400000000002</v>
       </c>
-      <c r="F7">
-        <f>E3:E7</f>
+      <c r="F8">
+        <f>E4:E8</f>
         <v>2.1216400000000002</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>2.120444</v>
       </c>
-      <c r="H7">
-        <f>G3:G7</f>
+      <c r="H8">
+        <f>G4:G8</f>
         <v>2.120444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>4.222334</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2.1342910000000002</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>2.1319159999999999</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>2.132457</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>4.2081850000000003</v>
+        <v>4.222334</v>
       </c>
       <c r="C12">
-        <v>2.1290909999999998</v>
+        <v>2.1342910000000002</v>
       </c>
       <c r="E12">
-        <v>2.1263839999999998</v>
+        <v>2.1319159999999999</v>
       </c>
       <c r="G12">
-        <v>2.127856</v>
+        <v>2.132457</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>4.2201599999999999</v>
+        <v>4.2081850000000003</v>
       </c>
       <c r="C13">
-        <v>2.1300340000000002</v>
+        <v>2.1290909999999998</v>
       </c>
       <c r="E13">
-        <v>2.127758</v>
+        <v>2.1263839999999998</v>
       </c>
       <c r="G13">
-        <v>2.1278570000000001</v>
+        <v>2.127856</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
-        <v>4.2083240000000002</v>
+        <v>4.2201599999999999</v>
       </c>
       <c r="C14">
-        <v>2.12243</v>
+        <v>2.1300340000000002</v>
       </c>
       <c r="E14">
-        <v>2.1265800000000001</v>
+        <v>2.127758</v>
       </c>
       <c r="G14">
-        <v>2.1252360000000001</v>
+        <v>2.1278570000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
+        <v>4.2083240000000002</v>
+      </c>
+      <c r="C15">
+        <v>2.12243</v>
+      </c>
+      <c r="E15">
+        <v>2.1265800000000001</v>
+      </c>
+      <c r="G15">
+        <v>2.1252360000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
         <v>4.2107270000000003</v>
       </c>
-      <c r="B15">
-        <f>A11:A15</f>
+      <c r="B16">
+        <f>A12:A16</f>
         <v>4.2107270000000003</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>2.1209600000000002</v>
       </c>
-      <c r="D15">
-        <f>C11:C15</f>
+      <c r="D16">
+        <f>C12:C16</f>
         <v>2.1209600000000002</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>2.1236600000000001</v>
       </c>
-      <c r="F15">
-        <f>E11:E15</f>
+      <c r="F16">
+        <f>E12:E16</f>
         <v>2.1236600000000001</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>2.127999</v>
       </c>
-      <c r="H15">
-        <f>G11:G15</f>
+      <c r="H16">
+        <f>G12:G16</f>
         <v>2.127999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="G19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>8.3901690000000002</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>2.140355</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>2.140606</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>2.1514929999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>8.3857809999999997</v>
+        <v>8.3901690000000002</v>
       </c>
       <c r="C21">
-        <v>2.1380560000000002</v>
+        <v>2.140355</v>
       </c>
       <c r="E21">
-        <v>2.1399050000000002</v>
+        <v>2.140606</v>
       </c>
       <c r="G21">
-        <v>2.1390229999999999</v>
+        <v>2.1514929999999999</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>8.3821349999999999</v>
+        <v>8.3857809999999997</v>
       </c>
       <c r="C22">
-        <v>2.139481</v>
+        <v>2.1380560000000002</v>
       </c>
       <c r="E22">
-        <v>2.1341100000000002</v>
+        <v>2.1399050000000002</v>
       </c>
       <c r="G22">
-        <v>2.1368019999999999</v>
+        <v>2.1390229999999999</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>8.3843169999999994</v>
+        <v>8.3821349999999999</v>
       </c>
       <c r="C23">
-        <v>2.1326369999999999</v>
+        <v>2.139481</v>
       </c>
       <c r="E23">
-        <v>2.1306600000000002</v>
+        <v>2.1341100000000002</v>
       </c>
       <c r="G23">
-        <v>2.1358090000000001</v>
+        <v>2.1368019999999999</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
+        <v>8.3843169999999994</v>
+      </c>
+      <c r="C24">
+        <v>2.1326369999999999</v>
+      </c>
+      <c r="E24">
+        <v>2.1306600000000002</v>
+      </c>
+      <c r="G24">
+        <v>2.1358090000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
         <v>8.3885059999999996</v>
       </c>
-      <c r="B24">
-        <f>A20:A24</f>
+      <c r="B25">
+        <f>A21:A25</f>
         <v>8.3885059999999996</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>2.1319370000000002</v>
       </c>
-      <c r="D24">
-        <f>AVERAGE(C20:C24)</f>
+      <c r="D25">
+        <f>AVERAGE(C21:C25)</f>
         <v>2.1364932000000003</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>2.1362570000000001</v>
       </c>
-      <c r="F24">
-        <f>E20:E24</f>
+      <c r="F25">
+        <f>E21:E25</f>
         <v>2.1362570000000001</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>2.1352669999999998</v>
       </c>
-      <c r="H24">
-        <f>G20:G24</f>
+      <c r="H25">
+        <f>G21:G25</f>
         <v>2.1352669999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27">
-        <v>16</v>
-      </c>
-      <c r="C27">
-        <v>16</v>
-      </c>
-      <c r="E27">
-        <v>16</v>
-      </c>
-      <c r="G27">
-        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>16.752087</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>2.1677909999999998</v>
+        <v>16</v>
       </c>
       <c r="E28">
-        <v>2.207837</v>
+        <v>16</v>
       </c>
       <c r="G28">
-        <v>2.2365780000000002</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>16.754024999999999</v>
+        <v>16.752087</v>
       </c>
       <c r="C29">
-        <v>2.1599439999999999</v>
+        <v>2.1677909999999998</v>
       </c>
       <c r="E29">
-        <v>2.1555620000000002</v>
+        <v>2.207837</v>
       </c>
       <c r="G29">
-        <v>2.2158319999999998</v>
+        <v>2.2365780000000002</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>16.754795000000001</v>
+        <v>16.754024999999999</v>
       </c>
       <c r="C30">
-        <v>2.1534990000000001</v>
+        <v>2.1599439999999999</v>
       </c>
       <c r="E30">
-        <v>2.1528420000000001</v>
+        <v>2.1555620000000002</v>
       </c>
       <c r="G30">
-        <v>2.1801879999999998</v>
+        <v>2.2158319999999998</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>16.748601000000001</v>
+        <v>16.754795000000001</v>
       </c>
       <c r="C31">
-        <v>2.149159</v>
+        <v>2.1534990000000001</v>
       </c>
       <c r="E31">
-        <v>2.1523560000000002</v>
+        <v>2.1528420000000001</v>
       </c>
       <c r="G31">
-        <v>2.1672410000000002</v>
+        <v>2.1801879999999998</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
+        <v>16.748601000000001</v>
+      </c>
+      <c r="C32">
+        <v>2.149159</v>
+      </c>
+      <c r="E32">
+        <v>2.1523560000000002</v>
+      </c>
+      <c r="G32">
+        <v>2.1672410000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
         <v>16.758751</v>
       </c>
-      <c r="B32">
-        <f>A28:A32</f>
+      <c r="B33">
+        <f>A29:A33</f>
         <v>16.758751</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>2.1557819999999999</v>
       </c>
-      <c r="D32">
-        <f>+AVERAGE(C28:C32)</f>
+      <c r="D33">
+        <f>+AVERAGE(C29:C33)</f>
         <v>2.157235</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>2.154868</v>
       </c>
-      <c r="F32">
-        <f>E28:E32</f>
+      <c r="F33">
+        <f>E29:E33</f>
         <v>2.154868</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>2.1626189999999998</v>
       </c>
-      <c r="H32">
-        <f>G28:G32</f>
+      <c r="H33">
+        <f>G29:G33</f>
         <v>2.1626189999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36">
-        <v>32</v>
-      </c>
-      <c r="C36">
-        <v>32</v>
-      </c>
-      <c r="E36">
-        <v>32</v>
-      </c>
-      <c r="G36">
-        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>33.522022</v>
+        <v>32</v>
       </c>
       <c r="C37">
-        <v>2.4036219999999999</v>
+        <v>32</v>
       </c>
       <c r="E37">
-        <v>2.266896</v>
+        <v>32</v>
       </c>
       <c r="G37">
-        <v>2.3187929999999999</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>33.475338000000001</v>
+        <v>33.522022</v>
       </c>
       <c r="C38">
-        <v>2.442688</v>
+        <v>2.4036219999999999</v>
       </c>
       <c r="E38">
-        <v>2.2285029999999999</v>
+        <v>2.266896</v>
       </c>
       <c r="G38">
-        <v>2.2798389999999999</v>
+        <v>2.3187929999999999</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>33.463346000000001</v>
+        <v>33.475338000000001</v>
       </c>
       <c r="C39">
-        <v>2.2717890000000001</v>
+        <v>2.442688</v>
       </c>
       <c r="E39">
-        <v>2.1941769999999998</v>
+        <v>2.2285029999999999</v>
       </c>
       <c r="G39">
-        <v>2.2402389999999999</v>
+        <v>2.2798389999999999</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>33.461804999999998</v>
+        <v>33.463346000000001</v>
       </c>
       <c r="C40">
-        <v>2.30606</v>
+        <v>2.2717890000000001</v>
       </c>
       <c r="E40">
-        <v>2.1835089999999999</v>
+        <v>2.1941769999999998</v>
       </c>
       <c r="G40">
-        <v>2.2236349999999998</v>
+        <v>2.2402389999999999</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
+        <v>33.461804999999998</v>
+      </c>
+      <c r="C41">
+        <v>2.30606</v>
+      </c>
+      <c r="E41">
+        <v>2.1835089999999999</v>
+      </c>
+      <c r="G41">
+        <v>2.2236349999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
         <v>33.472478000000002</v>
       </c>
-      <c r="B41">
-        <f>A37:A41</f>
+      <c r="B42">
+        <f>A38:A42</f>
         <v>33.472478000000002</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>2.267258</v>
       </c>
-      <c r="D41">
-        <f>AVERAGE(C37:C41)</f>
+      <c r="D42">
+        <f>AVERAGE(C38:C42)</f>
         <v>2.3382833999999999</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>2.2784230000000001</v>
       </c>
-      <c r="F41">
-        <f>E37:E41</f>
+      <c r="F42">
+        <f>E38:E42</f>
         <v>2.2784230000000001</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>2.2856239999999999</v>
       </c>
-      <c r="H41">
-        <f>G37:G41</f>
+      <c r="H42">
+        <f>G38:G42</f>
         <v>2.2856239999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46">
-        <v>64</v>
-      </c>
-      <c r="C46">
-        <v>64</v>
-      </c>
-      <c r="E46">
-        <v>64</v>
-      </c>
-      <c r="G46">
-        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
-        <v>66.939031</v>
+        <v>64</v>
       </c>
       <c r="C47">
-        <v>2.593378</v>
+        <v>64</v>
       </c>
       <c r="E47">
-        <v>2.3070189999999999</v>
+        <v>64</v>
       </c>
       <c r="G47">
-        <v>2.6852330000000002</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
-        <v>66.987172999999999</v>
+        <v>66.939031</v>
       </c>
       <c r="C48">
-        <v>2.5682140000000002</v>
+        <v>2.593378</v>
       </c>
       <c r="E48">
-        <v>2.2628460000000001</v>
+        <v>2.3070189999999999</v>
       </c>
       <c r="G48">
-        <v>2.5352839999999999</v>
+        <v>2.6852330000000002</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49">
-        <v>66.962649999999996</v>
+        <v>66.987172999999999</v>
       </c>
       <c r="C49">
-        <v>2.5535990000000002</v>
+        <v>2.5682140000000002</v>
       </c>
       <c r="E49">
-        <v>2.231846</v>
+        <v>2.2628460000000001</v>
       </c>
       <c r="G49">
-        <v>2.491832</v>
+        <v>2.5352839999999999</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
-        <v>66.989890000000003</v>
+        <v>66.962649999999996</v>
       </c>
       <c r="C50">
-        <v>2.4926599999999999</v>
+        <v>2.5535990000000002</v>
       </c>
       <c r="E50">
-        <v>2.2268729999999999</v>
+        <v>2.231846</v>
       </c>
       <c r="G50">
-        <v>2.4906830000000002</v>
+        <v>2.491832</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51">
+        <v>66.989890000000003</v>
+      </c>
+      <c r="C51">
+        <v>2.4926599999999999</v>
+      </c>
+      <c r="E51">
+        <v>2.2268729999999999</v>
+      </c>
+      <c r="G51">
+        <v>2.4906830000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
         <v>66.959328999999997</v>
       </c>
-      <c r="B51">
-        <f>A47:A51</f>
+      <c r="B52">
+        <f>A48:A52</f>
         <v>66.959328999999997</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>2.3802469999999998</v>
       </c>
-      <c r="D51">
-        <f>+AVERAGE(C47:C51)</f>
+      <c r="D52">
+        <f>+AVERAGE(C48:C52)</f>
         <v>2.5176196000000006</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <v>2.275712</v>
       </c>
-      <c r="F51">
-        <f>E47:E51</f>
+      <c r="F52">
+        <f>E48:E52</f>
         <v>2.275712</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>2.4855770000000001</v>
       </c>
-      <c r="H51">
-        <f>G47:G51</f>
+      <c r="H52">
+        <f>G48:G52</f>
         <v>2.4855770000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55">
+    <row r="56" spans="1:8">
+      <c r="A56">
         <v>128</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>128</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>128</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>128</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="C56">
-        <v>2.7383030000000002</v>
-      </c>
-      <c r="E56">
-        <v>2.4602550000000001</v>
-      </c>
-      <c r="G56">
-        <v>2.911883</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="C57">
-        <v>2.7150219999999998</v>
+        <v>2.7383030000000002</v>
       </c>
       <c r="E57">
-        <v>2.4081760000000001</v>
+        <v>2.4602550000000001</v>
       </c>
       <c r="G57">
-        <v>2.8365969999999998</v>
+        <v>2.911883</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="C58">
-        <v>2.5858340000000002</v>
+        <v>2.7150219999999998</v>
       </c>
       <c r="E58">
-        <v>2.460836</v>
+        <v>2.4081760000000001</v>
       </c>
       <c r="G58">
-        <v>2.8186870000000002</v>
+        <v>2.8365969999999998</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="C59">
-        <v>2.7002830000000002</v>
+        <v>2.5858340000000002</v>
       </c>
       <c r="E59">
-        <v>2.3688280000000002</v>
+        <v>2.460836</v>
       </c>
       <c r="G59">
-        <v>2.7883740000000001</v>
+        <v>2.8186870000000002</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="C60">
+        <v>2.7002830000000002</v>
+      </c>
+      <c r="E60">
+        <v>2.3688280000000002</v>
+      </c>
+      <c r="G60">
+        <v>2.7883740000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="C61">
         <v>2.785514</v>
       </c>
-      <c r="D60">
-        <f>AVERAGE(C56:C60)</f>
+      <c r="D61">
+        <f>AVERAGE(C57:C61)</f>
         <v>2.7049911999999998</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <v>2.3605999999999998</v>
       </c>
-      <c r="F60">
-        <f>AVERAGE(E56:E60)</f>
+      <c r="F61">
+        <f>AVERAGE(E57:E61)</f>
         <v>2.4117389999999999</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <v>2.7975469999999998</v>
       </c>
-      <c r="H60">
-        <f>AVERAGE(G56:G60)</f>
+      <c r="H61">
+        <f>AVERAGE(G57:G61)</f>
         <v>2.8306175999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64">
+    <row r="65" spans="1:9">
+      <c r="A65">
         <v>256</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>256</v>
       </c>
-      <c r="E64">
+      <c r="E65">
         <v>256</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>256</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
-      <c r="C65">
+    <row r="66" spans="1:9">
+      <c r="C66">
         <v>3.3193389999999998</v>
       </c>
-      <c r="E65">
+      <c r="E66">
         <v>2.9188190000000001</v>
       </c>
-      <c r="G65">
-        <v>4.4759950000000002</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="C66">
+      <c r="G66">
+        <v>4.2004279999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="C67">
         <v>3.043612</v>
       </c>
-      <c r="E66">
+      <c r="E67">
         <v>2.823677</v>
       </c>
-      <c r="G66">
-        <v>4.3768900000000004</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="C67">
+      <c r="G67">
+        <v>4.6538209999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="C68">
         <v>3.0856759999999999</v>
       </c>
-      <c r="E67">
+      <c r="E68">
         <v>2.797444</v>
       </c>
-      <c r="G67">
-        <v>4.384836</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="C68">
+      <c r="G68">
+        <v>3.882711</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="C69">
         <v>3.0053130000000001</v>
       </c>
-      <c r="E68">
+      <c r="E69">
         <v>2.792335</v>
       </c>
-      <c r="G68">
-        <v>4.2711610000000002</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="C69">
+      <c r="G69">
+        <v>3.875048</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="C70">
         <v>3.0639470000000002</v>
       </c>
-      <c r="D69">
-        <f>AVERAGE(C65:C69)</f>
+      <c r="D70">
+        <f>AVERAGE(C66:C70)</f>
         <v>3.1035773999999998</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <v>2.8671180000000001</v>
       </c>
-      <c r="F69">
-        <f>AVERAGE(E65:E69)</f>
+      <c r="F70">
+        <f>AVERAGE(E66:E70)</f>
         <v>2.8398785999999996</v>
       </c>
-      <c r="G69">
-        <v>4.2126650000000003</v>
-      </c>
-      <c r="H69">
-        <f>AVERAGE(G65:G69)</f>
-        <v>4.3443094000000002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72">
+      <c r="G70">
+        <v>3.896166</v>
+      </c>
+      <c r="H70">
+        <f>AVERAGE(G66:G70)</f>
+        <v>4.1016348000000002</v>
+      </c>
+      <c r="I70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73">
         <v>512</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>512</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <v>512</v>
       </c>
-      <c r="G72">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="C73">
+      <c r="G73">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="C74">
         <v>4.3758090000000003</v>
       </c>
-      <c r="E73">
-        <v>4.1020620000000001</v>
-      </c>
-      <c r="G73">
-        <v>11.789846000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="C74">
+      <c r="E74">
+        <v>4.4016060000000001</v>
+      </c>
+      <c r="G74">
+        <v>7.3288479999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="C75">
         <v>4.4047790000000004</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>4.27149</v>
       </c>
-      <c r="G74">
-        <v>11.879471000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="C75">
+      <c r="G75">
+        <v>6.5865590000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="C76">
         <v>3.3412269999999999</v>
       </c>
-      <c r="E75">
+      <c r="E76">
         <v>4.251881</v>
       </c>
-      <c r="G75">
-        <v>11.281983</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="C76">
+      <c r="G76">
+        <v>7.1269020000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="C77">
         <v>3.401853</v>
       </c>
-      <c r="E76">
+      <c r="E77">
         <v>4.1337190000000001</v>
       </c>
-      <c r="G76">
-        <v>11.649514</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="C77">
+      <c r="G77">
+        <v>8.4429839999999992</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="C78">
         <v>4.3321620000000003</v>
       </c>
-      <c r="D77">
-        <f>C73:C77</f>
+      <c r="D78">
+        <f>C74:C78</f>
         <v>4.3321620000000003</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>4.0621340000000004</v>
       </c>
-      <c r="F77">
-        <f>E73:E77</f>
+      <c r="F78">
+        <f>E74:E78</f>
         <v>4.0621340000000004</v>
       </c>
-      <c r="G77">
-        <v>11.556595</v>
-      </c>
-      <c r="H77">
-        <f>AVERAGE(G73:G77)</f>
-        <v>11.6314818</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80">
+      <c r="G78">
+        <v>6.588565</v>
+      </c>
+      <c r="H78">
+        <f>AVERAGE(G74:G78)</f>
+        <v>7.2147716000000006</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81">
         <v>1024</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>1024</v>
       </c>
-      <c r="E80">
+      <c r="E81">
         <v>1024</v>
       </c>
-      <c r="G80">
+      <c r="G81">
         <v>1024</v>
       </c>
     </row>
-    <row r="81" spans="3:8">
-      <c r="C81">
-        <v>15.813917999999999</v>
-      </c>
-      <c r="E81">
-        <v>8.8218499999999995</v>
-      </c>
-      <c r="G81">
+    <row r="82" spans="1:8">
+      <c r="C82">
+        <v>10.484881</v>
+      </c>
+      <c r="E82">
+        <v>6.3858779999999999</v>
+      </c>
+      <c r="G82">
         <v>42.714317000000001</v>
       </c>
     </row>
-    <row r="82" spans="3:8">
-      <c r="C82">
-        <v>15.13039</v>
-      </c>
-      <c r="E82">
-        <v>9.6352949999999993</v>
-      </c>
-      <c r="G82">
+    <row r="83" spans="1:8">
+      <c r="C83">
+        <v>10.887937000000001</v>
+      </c>
+      <c r="E83">
+        <v>7.3895039999999996</v>
+      </c>
+      <c r="G83">
         <v>43.014736999999997</v>
       </c>
     </row>
-    <row r="83" spans="3:8">
-      <c r="C83">
-        <v>16.477553</v>
-      </c>
-      <c r="E83">
-        <v>9.2685440000000003</v>
-      </c>
-      <c r="G83">
+    <row r="84" spans="1:8">
+      <c r="C84">
+        <v>11.556111</v>
+      </c>
+      <c r="E84">
+        <v>6.9166259999999999</v>
+      </c>
+      <c r="G84">
         <v>45.645094999999998</v>
       </c>
     </row>
-    <row r="84" spans="3:8">
-      <c r="C84">
-        <v>16.207439999999998</v>
-      </c>
-      <c r="E84">
-        <v>9.4351260000000003</v>
-      </c>
-      <c r="G84">
+    <row r="85" spans="1:8">
+      <c r="C85">
+        <v>9.322241</v>
+      </c>
+      <c r="E85">
+        <v>7.5339720000000003</v>
+      </c>
+      <c r="G85">
         <v>44.467646999999999</v>
       </c>
     </row>
-    <row r="85" spans="3:8">
-      <c r="C85">
-        <v>15.845494</v>
-      </c>
-      <c r="D85">
-        <f>C81:C85</f>
-        <v>15.845494</v>
-      </c>
-      <c r="E85">
-        <v>9.3378180000000004</v>
-      </c>
-      <c r="F85">
-        <f>E81:E85</f>
-        <v>9.3378180000000004</v>
-      </c>
-      <c r="G85">
+    <row r="86" spans="1:8">
+      <c r="C86">
+        <v>10.846582</v>
+      </c>
+      <c r="D86">
+        <f>AVERAGE(C82:C86)</f>
+        <v>10.6195504</v>
+      </c>
+      <c r="E86">
+        <v>7.5411760000000001</v>
+      </c>
+      <c r="F86">
+        <f>AVERAGE(E82:E86)</f>
+        <v>7.1534312</v>
+      </c>
+      <c r="G86">
         <v>43.672925999999997</v>
       </c>
-      <c r="H85">
-        <f>+AVERAGE(G81:G85)</f>
+      <c r="H86">
+        <f>+AVERAGE(G82:G86)</f>
         <v>43.902944399999996</v>
       </c>
     </row>
-    <row r="87" spans="3:8">
-      <c r="C87" t="s">
+    <row r="88" spans="1:8">
+      <c r="C88" t="s">
         <v>17</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E88" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="89" spans="1:8">
+      <c r="C89" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A7"/>
+  <autoFilter ref="A2:A8"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5382,8 +5465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5392,6 +5475,7 @@
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.6640625" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5647,7 +5731,7 @@
         <v>4.3321620000000003</v>
       </c>
       <c r="K33">
-        <v>15.845494</v>
+        <v>10.6195504</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -5787,10 +5871,10 @@
         <v>4.0621340000000004</v>
       </c>
       <c r="K55">
-        <v>9.3378180000000004</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
+        <v>7.1534312</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -5819,13 +5903,10 @@
         <v>256</v>
       </c>
       <c r="J76">
-        <v>512</v>
-      </c>
-      <c r="K76">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -5854,13 +5935,10 @@
         <v>5.5248493999999999</v>
       </c>
       <c r="J77">
-        <v>7.2896678000000001</v>
-      </c>
-      <c r="K77">
-        <v>11.8032056</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
+        <v>7.3069930000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -5889,13 +5967,10 @@
         <v>2.6043186</v>
       </c>
       <c r="J78">
-        <v>3.1656578</v>
-      </c>
-      <c r="K78">
-        <v>5.1867571999999997</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
+        <v>3.1429132000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -5921,13 +5996,10 @@
         <v>2.8306176000000001</v>
       </c>
       <c r="I79">
-        <v>4.3443094000000002</v>
+        <v>4.1016348000000002</v>
       </c>
       <c r="J79">
-        <v>11.6314818</v>
-      </c>
-      <c r="K79">
-        <v>43.902944400000003</v>
+        <v>7.2147715999999997</v>
       </c>
     </row>
     <row r="100" spans="3:3">
@@ -5950,10 +6022,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5963,62 +6035,114 @@
     <col min="3" max="3" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>32</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>64</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>3.7698580000000002</v>
+      </c>
+      <c r="B14">
+        <v>3.363359</v>
+      </c>
+      <c r="C14">
+        <v>2.3953769999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>128</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>4.1959229999999996</v>
+      </c>
+      <c r="B22">
+        <v>3.740316</v>
+      </c>
+      <c r="C22">
+        <v>3.08528</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>256</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>256</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>4.2850619999999999</v>
+      </c>
+      <c r="B30">
+        <v>5.2216810000000002</v>
+      </c>
+      <c r="C30">
+        <v>5.7828080000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>512</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>512</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>7.9109569999999998</v>
+      </c>
+      <c r="B39">
+        <v>7.9082840000000001</v>
+      </c>
+      <c r="C39">
+        <v>7.885529</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>1024</v>
+      </c>
+      <c r="D47">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -6037,7 +6161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -6050,20 +6174,20 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
bottleneck for large scale case
</commit_message>
<xml_diff>
--- a/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
+++ b/latex/eventWorkflow/eventdriven_experiments/microbench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="swift" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>chained</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
   </si>
   <si>
     <t>size of graph 9.6*6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>multinode node number 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -144,6 +140,34 @@
     <t>the sockets number get to the upper limitation(14:Socket closed)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>node1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multinode node number 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>512(total 1536)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256(total 768)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128(total 384)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -201,8 +225,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -419,7 +475,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="245">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -527,6 +583,22 @@
     <cellStyle name="访问过的超链接" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -633,6 +705,22 @@
     <cellStyle name="超链接" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="243" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2058,6 +2146,238 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>node1</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>multinodes!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128(total 384)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256(total 768)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512(total 1536)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>multinodes!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.769858</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.195923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.285062</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.910957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>node2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>multinodes!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128(total 384)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256(total 768)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512(total 1536)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>multinodes!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.363359</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.740316</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.221681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.908284</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>node3</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>multinodes!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128(total 384)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256(total 768)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512(total 1536)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>multinodes!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.395377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.08528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.782808</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.885529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2077978488"/>
+        <c:axId val="-2061611864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2077978488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2061611864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2061611864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077978488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -2190,6 +2510,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3479,7 +3834,7 @@
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4466,7 +4821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView topLeftCell="D47" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
@@ -4482,16 +4837,16 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5270,7 +5625,7 @@
         <v>4.1016348000000002</v>
       </c>
       <c r="I70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -5437,15 +5792,15 @@
     </row>
     <row r="88" spans="1:8">
       <c r="C88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="C89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -5465,8 +5820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6022,133 +6377,138 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>3.7698580000000002</v>
+      </c>
+      <c r="C5">
+        <v>4.1959229999999996</v>
+      </c>
       <c r="D5">
+        <v>4.2850619999999999</v>
+      </c>
+      <c r="E5">
+        <v>7.9109569999999998</v>
+      </c>
+      <c r="N5">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>3.363359</v>
+      </c>
+      <c r="C6">
+        <v>3.740316</v>
+      </c>
+      <c r="D6">
+        <v>5.2216810000000002</v>
+      </c>
+      <c r="E6">
+        <v>7.9082840000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>2.3953769999999999</v>
+      </c>
+      <c r="C7">
+        <v>3.08528</v>
+      </c>
+      <c r="D7">
+        <v>5.7828080000000002</v>
+      </c>
+      <c r="E7">
+        <v>7.885529</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="N13">
         <v>64</v>
       </c>
-      <c r="D13">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>3.7698580000000002</v>
-      </c>
-      <c r="B14">
-        <v>3.363359</v>
-      </c>
-      <c r="C14">
-        <v>2.3953769999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
+    </row>
+    <row r="21" spans="14:14">
+      <c r="N21">
         <v>128</v>
       </c>
-      <c r="D21">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>4.1959229999999996</v>
-      </c>
-      <c r="B22">
-        <v>3.740316</v>
-      </c>
-      <c r="C22">
-        <v>3.08528</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
+    </row>
+    <row r="29" spans="14:14">
+      <c r="N29">
         <v>256</v>
       </c>
-      <c r="D29">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>4.2850619999999999</v>
-      </c>
-      <c r="B30">
-        <v>5.2216810000000002</v>
-      </c>
-      <c r="C30">
-        <v>5.7828080000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
+    </row>
+    <row r="38" spans="2:14">
+      <c r="N38">
         <v>512</v>
       </c>
-      <c r="D38">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39">
-        <v>7.9109569999999998</v>
-      </c>
-      <c r="B39">
-        <v>7.9082840000000001</v>
-      </c>
-      <c r="C39">
-        <v>7.885529</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47">
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47">
         <v>1024</v>
       </c>
-      <c r="D47">
+      <c r="N47">
         <v>1024</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
-        <v>28</v>
+    <row r="48" spans="2:14">
+      <c r="B48" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6162,7 +6522,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6174,20 +6534,20 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>